<commit_message>
Added alias for R245fa
</commit_message>
<xml_diff>
--- a/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
+++ b/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="418">
   <si>
     <t>1BUTENE</t>
   </si>
@@ -1304,6 +1304,9 @@
   </si>
   <si>
     <t>Tcrit</t>
+  </si>
+  <si>
+    <t>R245fa</t>
   </si>
 </sst>
 </file>
@@ -2586,9 +2589,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D108" sqref="D108"/>
+      <selection pane="topRight" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10341,11 +10344,11 @@
         <v>153</v>
       </c>
       <c r="C100" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D100" s="16" t="e">
+        <v>417</v>
+      </c>
+      <c r="D100" s="16">
         <f>[1]!Props1(C100,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>427.16</v>
       </c>
       <c r="E100" s="16" t="s">
         <v>259</v>

</xml_diff>

<commit_message>
Adding environmental data on fluids from DTU - need to rework the input from file
</commit_message>
<xml_diff>
--- a/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
+++ b/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="10005" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="420">
   <si>
     <t>1BUTENE</t>
   </si>
@@ -1307,6 +1307,12 @@
   </si>
   <si>
     <t>R245fa</t>
+  </si>
+  <si>
+    <t>OrthoHydrogen</t>
+  </si>
+  <si>
+    <t>ParaHydrogen</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1612,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1737,6 +1743,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2035,7 +2047,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2181,6 +2193,13 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2589,17 +2608,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="825" topLeftCell="A56" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="4" customWidth="1"/>
+    <col min="4" max="4" width="101.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -2644,20 +2663,20 @@
       <c r="H1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
       <c r="L1" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
       <c r="Q1" s="29" t="s">
         <v>124</v>
       </c>
@@ -3226,9 +3245,9 @@
       <c r="C9" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="D9" s="16" t="e">
+      <c r="D9" s="16">
         <f>[1]!Props1(C9,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>562.02</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="11" t="s">
@@ -3460,9 +3479,9 @@
         <v>166</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="16" t="e">
+      <c r="D12" s="16" t="str">
         <f>[1]!Props1(C12,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16" t="s">
@@ -3612,9 +3631,9 @@
         <v>167</v>
       </c>
       <c r="C14" s="16"/>
-      <c r="D14" s="16" t="e">
+      <c r="D14" s="16" t="str">
         <f>[1]!Props1(C14,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="11" t="s">
@@ -3688,9 +3707,9 @@
         <v>168</v>
       </c>
       <c r="C15" s="16"/>
-      <c r="D15" s="16" t="e">
+      <c r="D15" s="16" t="str">
         <f>[1]!Props1(C15,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16">
@@ -3764,9 +3783,9 @@
         <v>169</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="16" t="e">
+      <c r="D16" s="16" t="str">
         <f>[1]!Props1(C16,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16">
@@ -3840,9 +3859,9 @@
         <v>170</v>
       </c>
       <c r="C17" s="16"/>
-      <c r="D17" s="16" t="e">
+      <c r="D17" s="16" t="str">
         <f>[1]!Props1(C17,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="11" t="s">
@@ -4308,9 +4327,9 @@
       <c r="C23" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="D23" s="16" t="e">
+      <c r="D23" s="16">
         <f>[1]!Props1(C23,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>398.3</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="11" t="s">
@@ -4386,9 +4405,9 @@
       <c r="C24" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="D24" s="16" t="e">
+      <c r="D24" s="16" t="str">
         <f>[1]!Props1(C24,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [Deuterium] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16">
@@ -4464,9 +4483,9 @@
       <c r="C25" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="D25" s="16" t="e">
+      <c r="D25" s="16" t="str">
         <f>[1]!Props1(C25,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [DeuteriumOxide] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
@@ -5090,7 +5109,7 @@
       </c>
       <c r="D33" s="16">
         <f>[1]!Props1(C33,"Tcrit")</f>
-        <v>513.9</v>
+        <v>514.71</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16" t="s">
@@ -5246,9 +5265,9 @@
       <c r="C35" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="D35" s="16" t="e">
+      <c r="D35" s="16" t="str">
         <f>[1]!Props1(C35,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [Fluorine] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16" t="s">
@@ -5632,10 +5651,7 @@
         <v>112</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="16" t="e">
-        <f>[1]!Props1(C40,"Tcrit")</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="D40" s="16"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16" t="s">
         <v>112</v>
@@ -6012,7 +6028,7 @@
       </c>
       <c r="D45" s="16">
         <f>[1]!Props1(C45,"Tcrit")</f>
-        <v>407.81</v>
+        <v>407.81700000000001</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="11" t="s">
@@ -6546,9 +6562,9 @@
       <c r="C52" s="16" t="s">
         <v>389</v>
       </c>
-      <c r="D52" s="16" t="e">
+      <c r="D52" s="16" t="str">
         <f>[1]!Props1(C52,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [Methanol] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E52" s="16"/>
       <c r="F52" s="16" t="s">
@@ -6624,9 +6640,9 @@
       <c r="C53" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="D53" s="16" t="e">
+      <c r="D53" s="16">
         <f>[1]!Props1(C53,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>799</v>
       </c>
       <c r="E53" s="16"/>
       <c r="F53" s="14" t="s">
@@ -7170,9 +7186,9 @@
       <c r="C60" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="D60" s="16" t="e">
+      <c r="D60" s="16">
         <f>[1]!Props1(C60,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>44.491799999999998</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>231</v>
@@ -7328,9 +7344,9 @@
       <c r="C62" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="D62" s="16" t="e">
+      <c r="D62" s="16" t="str">
         <f>[1]!Props1(C62,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [NitrogenTrifluoride] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E62" s="16"/>
       <c r="F62" s="16">
@@ -7636,11 +7652,11 @@
         <v>159</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" s="16" t="e">
+        <v>418</v>
+      </c>
+      <c r="D66" s="16">
         <f>[1]!Props1(C66,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>33.22</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="16" t="s">
@@ -7792,11 +7808,11 @@
         <v>158</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D68" s="16" t="e">
+        <v>419</v>
+      </c>
+      <c r="D68" s="16">
         <f>[1]!Props1(C68,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>32.938000000000002</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="16" t="s">
@@ -8110,9 +8126,9 @@
       <c r="C72" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="D72" s="16" t="e">
+      <c r="D72" s="16" t="str">
         <f>[1]!Props1(C72,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [Propyne] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="11" t="s">
@@ -8178,85 +8194,85 @@
       <c r="Z72" s="7"/>
       <c r="AA72" s="7"/>
     </row>
-    <row r="73" spans="1:27">
-      <c r="A73" s="16" t="s">
+    <row r="73" spans="1:27" s="55" customFormat="1">
+      <c r="A73" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C73" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="D73" s="16" t="e">
+      <c r="D73" s="53">
         <f>[1]!Props1(C73,"Tcrit")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E73" s="16" t="s">
+        <v>471.06</v>
+      </c>
+      <c r="E73" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="F73" s="16">
+      <c r="F73" s="53">
         <v>6730</v>
       </c>
-      <c r="G73" s="16">
+      <c r="G73" s="53">
         <v>4750</v>
       </c>
-      <c r="H73" s="16">
+      <c r="H73" s="53">
         <v>1620</v>
       </c>
-      <c r="I73" s="16">
+      <c r="I73" s="53">
         <v>1</v>
       </c>
-      <c r="J73" s="16">
+      <c r="J73" s="53">
         <v>1</v>
       </c>
-      <c r="K73" s="16">
+      <c r="K73" s="53">
         <v>1</v>
       </c>
-      <c r="L73" s="10">
+      <c r="L73" s="53">
         <v>541</v>
       </c>
-      <c r="M73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="N73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="O73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="P73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="R73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="S73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="T73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="U73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="V73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="W73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="X73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z73" s="7"/>
-      <c r="AA73" s="7"/>
+      <c r="M73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="N73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="O73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="P73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="R73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="S73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="T73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="U73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="V73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="W73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="X73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y73" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z73" s="54"/>
+      <c r="AA73" s="54"/>
     </row>
     <row r="74" spans="1:27">
       <c r="A74" s="16" t="s">
@@ -8268,9 +8284,9 @@
       <c r="C74" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D74" s="16" t="e">
+      <c r="D74" s="16" t="str">
         <f>[1]!Props1(C74,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R113] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>236</v>
@@ -8348,9 +8364,9 @@
       <c r="C75" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D75" s="16" t="e">
+      <c r="D75" s="16" t="str">
         <f>[1]!Props1(C75,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R114] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>237</v>
@@ -8428,9 +8444,9 @@
       <c r="C76" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D76" s="16" t="e">
+      <c r="D76" s="16" t="str">
         <f>[1]!Props1(C76,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R115] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E76" s="16" t="s">
         <v>238</v>
@@ -8588,9 +8604,9 @@
       <c r="C78" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D78" s="16" t="e">
+      <c r="D78" s="16" t="str">
         <f>[1]!Props1(C78,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R12] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>240</v>
@@ -8908,9 +8924,9 @@
       <c r="C82" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="16" t="e">
+      <c r="D82" s="16">
         <f>[1]!Props1(C82,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>395.42500000000001</v>
       </c>
       <c r="E82" s="16" t="s">
         <v>243</v>
@@ -8988,9 +9004,9 @@
       <c r="C83" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D83" s="16" t="e">
+      <c r="D83" s="16">
         <f>[1]!Props1(C83,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>339.173</v>
       </c>
       <c r="E83" s="16" t="s">
         <v>244</v>
@@ -9068,9 +9084,9 @@
       <c r="C84" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="16" t="e">
+      <c r="D84" s="16" t="str">
         <f>[1]!Props1(C84,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R13] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E84" s="16" t="s">
         <v>245</v>
@@ -9228,9 +9244,9 @@
       <c r="C86" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="16" t="e">
+      <c r="D86" s="16" t="str">
         <f>[1]!Props1(C86,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R14] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E86" s="16" t="s">
         <v>247</v>
@@ -9308,9 +9324,9 @@
       <c r="C87" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="16" t="e">
+      <c r="D87" s="16" t="str">
         <f>[1]!Props1(C87,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R141B] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E87" s="16" t="s">
         <v>248</v>
@@ -9388,9 +9404,9 @@
       <c r="C88" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D88" s="16" t="e">
+      <c r="D88" s="16" t="str">
         <f>[1]!Props1(C88,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R142B] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E88" s="16" t="s">
         <v>249</v>
@@ -9550,7 +9566,7 @@
       </c>
       <c r="D90" s="16">
         <f>[1]!Props1(C90,"Tcrit")</f>
-        <v>386.41</v>
+        <v>386.411</v>
       </c>
       <c r="E90" s="16" t="s">
         <v>251</v>
@@ -9628,9 +9644,9 @@
       <c r="C91" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D91" s="16" t="e">
+      <c r="D91" s="16">
         <f>[1]!Props1(C91,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>375.25</v>
       </c>
       <c r="E91" s="16"/>
       <c r="F91" s="16" t="s">
@@ -9706,9 +9722,9 @@
       <c r="C92" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D92" s="16" t="e">
+      <c r="D92" s="16" t="str">
         <f>[1]!Props1(C92,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R21] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E92" s="16" t="s">
         <v>252</v>
@@ -10266,9 +10282,9 @@
       <c r="C99" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D99" s="16" t="e">
+      <c r="D99" s="16" t="str">
         <f>[1]!Props1(C99,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [R245CA] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E99" s="16" t="s">
         <v>258</v>
@@ -10506,9 +10522,9 @@
       <c r="C102" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D102" s="16" t="e">
+      <c r="D102" s="16">
         <f>[1]!Props1(C102,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>460</v>
       </c>
       <c r="E102" s="16" t="s">
         <v>261</v>
@@ -10986,9 +11002,9 @@
       <c r="C108" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D108" s="16" t="e">
+      <c r="D108" s="16" t="str">
         <f>[1]!Props1(C108,"Tcrit")</f>
-        <v>#VALUE!</v>
+        <v>CoolProp error: Your fluid name [RC318] is not a CoolProp fluid, a REFPROP fluid, a brine or a liquid</v>
       </c>
       <c r="E108" s="16" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
Environmental constants now loaded, except for ASHRAE 34, not clear how to do that...
</commit_message>
<xml_diff>
--- a/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
+++ b/Vault/addInfoDTU/environmental_impact_version_28032013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="10005" windowHeight="5835"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="10005" windowHeight="5775"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2609,8 +2609,8 @@
   <dimension ref="A1:AA146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="825" topLeftCell="A56" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="825" topLeftCell="A41" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>